<commit_message>
update tien xu ly
</commit_message>
<xml_diff>
--- a/TienXuLy.xlsx
+++ b/TienXuLy.xlsx
@@ -1325,9 +1325,6 @@
     <t>Xin hỏi mức giá 44,990 triệu là giá trả góp 0 đồng. Còn khi mua trực tiếp được trừ thêm 10% hả shop?</t>
   </si>
   <si>
-    <t>M k hài lòng sp iPhone 13promax 1t mua tại tgdd. Dung lượng máy 1T mà m cài thêm có Facebook, messenger, shopee mà còn trống giá 3.2gh. iPhone vừa chạy ios vừa chạy được ch play. Mới tải 3 ứng dụng trên ch play. Máy mua từ 12/21 mà như cục sắt. Lên YouTube xem thì báo bộ nhớ trong hết dung lượng yêu cầu làm trống bộ nhớ</t>
-  </si>
-  <si>
     <t>Sài mượt ok nhưng loa nghe cứ rè rè kiểu gì ấy</t>
   </si>
   <si>
@@ -1566,6 +1563,9 @@
   </si>
   <si>
     <t>Điện thoại mới mua , mà sao thao tác chậm quá , chức năng sữ lý quay lại chậm . chậm hơn cái nokia đời củ , cách đây 10 năm .</t>
+  </si>
+  <si>
+    <t>Mình không hài lòng sp iPhone 13promax 1t mua tại thế giới di động. Dung lượng máy 1T mà mình cài thêm có Facebook, messenger, shopee mà còn trống giá 3.2gh. iPhone vừa chạy ios vừa chạy được ch play. Mới tải 3 ứng dụng trên ch play. Máy mua từ 12/21 mà như cục sắt. Lên YouTube xem thì báo bộ nhớ trong hết dung lượng yêu cầu làm trống bộ nhớ</t>
   </si>
 </sst>
 </file>
@@ -1935,8 +1935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B528"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A292" workbookViewId="0">
-      <selection activeCell="A311" sqref="A311:XFD311"/>
+    <sheetView tabSelected="1" topLeftCell="A301" workbookViewId="0">
+      <selection activeCell="A310" sqref="A310"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2242,7 +2242,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>433</v>
+        <v>513</v>
       </c>
       <c r="B38" t="s">
         <v>7</v>
@@ -2274,7 +2274,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B42" t="s">
         <v>10</v>
@@ -2290,7 +2290,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B44" t="s">
         <v>10</v>
@@ -2314,7 +2314,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B47" t="s">
         <v>7</v>
@@ -2346,7 +2346,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B51" t="s">
         <v>7</v>
@@ -2370,7 +2370,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B54" t="s">
         <v>5</v>
@@ -2386,7 +2386,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B56" t="s">
         <v>10</v>
@@ -2402,7 +2402,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B58" t="s">
         <v>10</v>
@@ -2418,23 +2418,23 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B60" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
+    <row r="61" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B62" t="s">
         <v>5</v>
@@ -2450,7 +2450,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B64" t="s">
         <v>5</v>
@@ -2490,7 +2490,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B69" t="s">
         <v>7</v>
@@ -2522,7 +2522,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B73" t="s">
         <v>7</v>
@@ -2570,7 +2570,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B79" t="s">
         <v>7</v>
@@ -2610,7 +2610,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B84" t="s">
         <v>7</v>
@@ -2650,7 +2650,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B89" t="s">
         <v>5</v>
@@ -2674,7 +2674,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B92" t="s">
         <v>10</v>
@@ -2690,7 +2690,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B94" t="s">
         <v>7</v>
@@ -2714,7 +2714,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B97" t="s">
         <v>5</v>
@@ -2730,7 +2730,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B99" t="s">
         <v>10</v>
@@ -2778,7 +2778,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B105" t="s">
         <v>5</v>
@@ -2794,7 +2794,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B107" t="s">
         <v>7</v>
@@ -2810,7 +2810,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B109" t="s">
         <v>7</v>
@@ -2826,7 +2826,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B111" t="s">
         <v>10</v>
@@ -2882,7 +2882,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B118" t="s">
         <v>7</v>
@@ -2906,7 +2906,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B121" t="s">
         <v>10</v>
@@ -2930,7 +2930,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B124" t="s">
         <v>7</v>
@@ -2954,7 +2954,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B127" t="s">
         <v>10</v>
@@ -2978,7 +2978,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B130" t="s">
         <v>7</v>
@@ -2994,7 +2994,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B132" t="s">
         <v>7</v>
@@ -3010,7 +3010,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B134" t="s">
         <v>7</v>
@@ -3034,7 +3034,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B137" t="s">
         <v>7</v>
@@ -3074,7 +3074,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B142" t="s">
         <v>7</v>
@@ -3106,7 +3106,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B146" t="s">
         <v>7</v>
@@ -3130,7 +3130,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B149" t="s">
         <v>7</v>
@@ -3154,7 +3154,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B152" t="s">
         <v>10</v>
@@ -3178,7 +3178,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B155" t="s">
         <v>10</v>
@@ -3202,7 +3202,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B158" t="s">
         <v>10</v>
@@ -3218,7 +3218,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B160" t="s">
         <v>10</v>
@@ -3250,7 +3250,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B164" t="s">
         <v>10</v>
@@ -3266,7 +3266,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B166" t="s">
         <v>5</v>
@@ -3290,7 +3290,7 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B169" t="s">
         <v>7</v>
@@ -3306,7 +3306,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B171" t="s">
         <v>7</v>
@@ -3322,7 +3322,7 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B173" t="s">
         <v>7</v>
@@ -3338,7 +3338,7 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B175" t="s">
         <v>10</v>
@@ -3394,7 +3394,7 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B182" t="s">
         <v>10</v>
@@ -3442,7 +3442,7 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B188" t="s">
         <v>5</v>
@@ -3458,7 +3458,7 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B190" t="s">
         <v>7</v>
@@ -3482,7 +3482,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B193" t="s">
         <v>7</v>
@@ -3498,7 +3498,7 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B195" t="s">
         <v>5</v>
@@ -3522,7 +3522,7 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B198" t="s">
         <v>5</v>
@@ -3562,7 +3562,7 @@
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B203" t="s">
         <v>7</v>
@@ -3586,7 +3586,7 @@
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B206" t="s">
         <v>7</v>
@@ -3618,7 +3618,7 @@
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B210" t="s">
         <v>151</v>
@@ -3682,7 +3682,7 @@
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B218" t="s">
         <v>7</v>
@@ -3714,7 +3714,7 @@
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B222" t="s">
         <v>151</v>
@@ -3730,7 +3730,7 @@
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B224" t="s">
         <v>7</v>
@@ -3778,7 +3778,7 @@
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B230" t="s">
         <v>7</v>
@@ -3818,7 +3818,7 @@
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B235" t="s">
         <v>7</v>
@@ -3866,7 +3866,7 @@
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" s="3" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B241" t="s">
         <v>7</v>
@@ -3882,7 +3882,7 @@
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B243" t="s">
         <v>5</v>
@@ -3898,7 +3898,7 @@
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B245" t="s">
         <v>5</v>
@@ -3938,7 +3938,7 @@
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B250" t="s">
         <v>5</v>
@@ -3962,7 +3962,7 @@
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B253" t="s">
         <v>5</v>
@@ -3978,7 +3978,7 @@
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B255" t="s">
         <v>7</v>
@@ -3994,7 +3994,7 @@
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B257" t="s">
         <v>5</v>
@@ -4010,7 +4010,7 @@
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B259" t="s">
         <v>7</v>
@@ -4050,7 +4050,7 @@
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B264" t="s">
         <v>7</v>
@@ -4066,7 +4066,7 @@
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B266" t="s">
         <v>5</v>
@@ -4082,7 +4082,7 @@
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B268" t="s">
         <v>7</v>
@@ -4090,7 +4090,7 @@
     </row>
     <row r="269" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B269" s="5" t="s">
         <v>7</v>
@@ -4114,7 +4114,7 @@
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B272" t="s">
         <v>5</v>
@@ -4146,7 +4146,7 @@
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B276" t="s">
         <v>7</v>
@@ -4162,7 +4162,7 @@
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B278" t="s">
         <v>5</v>
@@ -4186,7 +4186,7 @@
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B281" t="s">
         <v>5</v>
@@ -4218,7 +4218,7 @@
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B285" t="s">
         <v>7</v>
@@ -4250,7 +4250,7 @@
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B289" t="s">
         <v>5</v>
@@ -4274,7 +4274,7 @@
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292" s="3" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B292" t="s">
         <v>7</v>
@@ -4290,7 +4290,7 @@
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B294" t="s">
         <v>5</v>
@@ -4322,7 +4322,7 @@
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B298" t="s">
         <v>7</v>
@@ -4354,7 +4354,7 @@
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B302" t="s">
         <v>7</v>
@@ -4370,7 +4370,7 @@
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A304" s="3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B304" t="s">
         <v>7</v>
@@ -4418,7 +4418,7 @@
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B310" t="s">
         <v>5</v>

</xml_diff>